<commit_message>
Adds test the shows bug with function counts
The cell SUM() + SUM() gets counted  twice for sums.  Not ideal.
</commit_message>
<xml_diff>
--- a/spreadsheet-analyzer/src/test/resources/small-worksheet.xlsx
+++ b/spreadsheet-analyzer/src/test/resources/small-worksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Downloads\Source\xlAnalysis\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,16 +367,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -392,7 +392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
@@ -415,7 +415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="C4">
         <v>1</v>
       </c>
@@ -454,7 +454,7 @@
         <v>43.58591579635798</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="B5">
         <v>1</v>
       </c>
@@ -510,7 +510,7 @@
         <v>27.499651112582431</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="B6">
         <v>2</v>
       </c>
@@ -569,7 +569,7 @@
         <v>21.79295789817899</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7">
         <v>3</v>
       </c>
@@ -629,7 +629,7 @@
         <v>18.771432195652185</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="B8">
         <v>4</v>
       </c>
@@ -685,7 +685,7 @@
         <v>16.861333881709434</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9">
         <v>5</v>
       </c>
@@ -741,7 +741,7 @@
         <v>15.525616463347786</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10">
         <v>6</v>
       </c>
@@ -797,7 +797,7 @@
         <v>14.528638598785994</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11">
         <v>7</v>
       </c>
@@ -853,7 +853,7 @@
         <v>13.749825556291215</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12">
         <v>8</v>
       </c>
@@ -909,7 +909,7 @@
         <v>13.12066804318829</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="B13">
         <v>9</v>
       </c>
@@ -965,7 +965,7 @@
         <v>12.599155179580302</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="B14">
         <v>10</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>12.157983741138205</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="B15">
         <v>11</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>11.778577443832342</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="B16">
         <v>12</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>11.447820518083693</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17">
         <v>13</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13202860761145</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="G19">
         <v>3.1415000000000002</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13">
       <c r="C23" s="2">
         <v>1234.56</v>
       </c>
@@ -1206,15 +1206,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:G6"/>
+  <dimension ref="E6:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:9">
       <c r="E6" s="1">
         <f>1+Sheet1!L19</f>
         <v>42078</v>
@@ -1222,6 +1222,10 @@
       <c r="G6">
         <f>COUNT(Sheet1!O1:P24)</f>
         <v>26</v>
+      </c>
+      <c r="I6">
+        <f>SUM(I3:M3) + SUM(K11:K16)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates tests to use proper division count
</commit_message>
<xml_diff>
--- a/spreadsheet-analyzer/src/test/resources/small-worksheet.xlsx
+++ b/spreadsheet-analyzer/src/test/resources/small-worksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Downloads\Source\xlAnalysis\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinLubick\Documents\CommonCrawler\spreadsheet-analyzer\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1133,7 +1133,7 @@
         <v>11.447820518083693</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:17">
       <c r="B17">
         <v>13</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>13202860761145</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:17">
       <c r="G19">
         <v>3.1415000000000002</v>
       </c>
@@ -1190,9 +1190,31 @@
         <v>42077</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="21" spans="2:17">
+      <c r="Q21">
+        <f>O4+O5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="Q22">
+        <f>O6/O7</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
       <c r="C23" s="2">
         <v>1234.56</v>
+      </c>
+      <c r="Q23">
+        <f>O8*O9</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="Q24">
+        <f>O9-O10</f>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1208,7 +1230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E6:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>